<commit_message>
Updated per club request
Updated Club ID and council rep for LSHR
Adjusted hours for LSR.
</commit_message>
<xml_diff>
--- a/NORTH TEXAS CLUB EXCEL SHEET.xlsx
+++ b/NORTH TEXAS CLUB EXCEL SHEET.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GIT\dfwtrainshows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F0415C-7145-4A2C-8F1B-31A06AE8E858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92096763-25E2-406D-B3D1-34451865E21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{BE3F0A9D-E83B-4903-A811-1F998F2D6180}"/>
+    <workbookView xWindow="29415" yWindow="495" windowWidth="21825" windowHeight="11475" xr2:uid="{BE3F0A9D-E83B-4903-A811-1F998F2D6180}"/>
   </bookViews>
   <sheets>
     <sheet name="Council" sheetId="1" r:id="rId1"/>
@@ -448,12 +448,6 @@
     <t>Richard Moore</t>
   </si>
   <si>
-    <t>LONE STAR HIGH RAILERS - LSTR</t>
-  </si>
-  <si>
-    <t>John Read</t>
-  </si>
-  <si>
     <t>Chris Atkins</t>
   </si>
   <si>
@@ -508,9 +502,6 @@
     <t>LSF</t>
   </si>
   <si>
-    <t>LSRT</t>
-  </si>
-  <si>
     <t>TRD</t>
   </si>
   <si>
@@ -560,6 +551,15 @@
   </si>
   <si>
     <t>ALL</t>
+  </si>
+  <si>
+    <t>LSHR</t>
+  </si>
+  <si>
+    <t>LONE STAR HIGH RAILERS - LSHR</t>
+  </si>
+  <si>
+    <t>Jim Shepherd</t>
   </si>
 </sst>
 </file>
@@ -678,7 +678,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -739,9 +739,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1062,8 +1059,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K201"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1106,17 +1103,17 @@
       <c r="K1" s="6"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
-        <v>176</v>
+      <c r="A2" s="5" t="s">
+        <v>173</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="8"/>
@@ -1133,10 +1130,10 @@
         <v>61</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>72</v>
@@ -1160,7 +1157,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>136</v>
@@ -1183,7 +1180,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>9</v>
@@ -1210,7 +1207,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>37</v>
@@ -1235,7 +1232,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>32</v>
@@ -1259,10 +1256,10 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>30</v>
@@ -1283,14 +1280,14 @@
       <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
-        <v>176</v>
+      <c r="A9" s="5" t="s">
+        <v>173</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>54</v>
@@ -1314,7 +1311,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>137</v>
@@ -1337,13 +1334,13 @@
         <v>8</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="8"/>
@@ -1357,10 +1354,10 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>31</v>
@@ -1386,10 +1383,10 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>36</v>
@@ -1418,10 +1415,10 @@
         <v>62</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>58</v>
@@ -1445,10 +1442,10 @@
         <v>62</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>69</v>
@@ -1472,7 +1469,7 @@
         <v>62</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>34</v>
@@ -1499,7 +1496,7 @@
         <v>62</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>35</v>
@@ -1524,7 +1521,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>20</v>
@@ -1551,7 +1548,7 @@
         <v>46</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>22</v>
@@ -1575,13 +1572,13 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>64</v>
@@ -1602,13 +1599,13 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>134</v>
@@ -1626,13 +1623,13 @@
         <v>46</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>139</v>
+        <v>175</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>140</v>
+        <v>176</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="8"/>
@@ -1649,7 +1646,7 @@
         <v>46</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>33</v>
@@ -1674,7 +1671,7 @@
         <v>63</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Update NORTH TEXAS CLUB EXCEL SHEET.xlsx
added last rep info
</commit_message>
<xml_diff>
--- a/NORTH TEXAS CLUB EXCEL SHEET.xlsx
+++ b/NORTH TEXAS CLUB EXCEL SHEET.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GIT\dfwtrainshows\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\dfwtrainshows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D37CB6-F04D-4281-81A9-11AB53484001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2538069B-4BCB-4BB9-BBAA-C07058DDEF6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{BE3F0A9D-E83B-4903-A811-1F998F2D6180}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BE3F0A9D-E83B-4903-A811-1F998F2D6180}"/>
   </bookViews>
   <sheets>
     <sheet name="Council" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="182">
   <si>
     <t>GUAGE</t>
   </si>
@@ -445,9 +445,6 @@
     <t>Richard Moore</t>
   </si>
   <si>
-    <t>LONE STAR rEGION - NMRA</t>
-  </si>
-  <si>
     <t>NMRA LONE STAR, DIVISION 3 -TRD</t>
   </si>
   <si>
@@ -566,6 +563,18 @@
   </si>
   <si>
     <t>Don30man@aol.com</t>
+  </si>
+  <si>
+    <t>NMRA LONE STAR, Division 1 - LSR</t>
+  </si>
+  <si>
+    <t>817)528-1546</t>
+  </si>
+  <si>
+    <t>(469237-5440)</t>
+  </si>
+  <si>
+    <t>jim.texasmodeltraincollections@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -643,7 +652,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -704,6 +713,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -718,7 +733,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -795,6 +810,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1113,659 +1137,667 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D210DD1-4B40-48B8-800F-0A70CB83221D}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K201"/>
+  <dimension ref="A1:K199"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A7" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="34.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="25.140625" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" style="1" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="1" max="2" width="11.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="25.109375" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" style="1" customWidth="1"/>
+    <col min="9" max="10" width="9.109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="7">
-        <v>8177157999</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="6"/>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="5"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>9</v>
+      <c r="B2" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>135</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E2" s="7">
-        <v>2147631593</v>
+        <v>8177157999</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>11</v>
+        <v>103</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>16</v>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>5</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>136</v>
+        <v>149</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>9</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>15</v>
+        <v>43</v>
+      </c>
+      <c r="E3" s="7">
+        <v>2147631593</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="23"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="C4" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="F4" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="23"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="F5" s="21" t="s">
+      <c r="E6" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="F6" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G6" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5" t="s">
-        <v>47</v>
-      </c>
+      <c r="H6" s="5"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>46</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>172</v>
+        <v>22</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="H7" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>169</v>
-      </c>
       <c r="C8" s="5" t="s">
-        <v>138</v>
+        <v>171</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="8"/>
+        <v>172</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>181</v>
+      </c>
       <c r="G8" s="8" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
-        <v>62</v>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>169</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>144</v>
+        <v>178</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>59</v>
+        <v>179</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>52</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>146</v>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
+        <v>62</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5">
-        <v>1950</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" s="5"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
-        <v>63</v>
+        <v>145</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>27</v>
+        <v>141</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="H11" s="5"/>
+        <v>65</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5">
+        <v>1950</v>
+      </c>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
-        <v>62</v>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
+        <v>63</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>143</v>
+        <v>27</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>61</v>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="18" t="s">
+        <v>62</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>145</v>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>155</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>134</v>
+        <v>139</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="5"/>
+        <v>81</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H14" s="5"/>
+      <c r="I14" s="6"/>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>161</v>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>144</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E15" s="7">
-        <v>9038152207</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="6"/>
+        <v>140</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="5"/>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
-        <v>148</v>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="E16" s="7">
-        <v>4693860824</v>
+        <v>9038152207</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>101</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>5</v>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="19" t="s">
+        <v>147</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>167</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="E17" s="7">
-        <v>2146753596</v>
+        <v>4693860824</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
+        <v>88</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>101</v>
+      </c>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E18" s="7">
-        <v>8176737092</v>
+        <v>2146753596</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>102</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
-        <v>62</v>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="13" t="s">
+        <v>5</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="E19" s="7">
-        <v>8177157999</v>
+        <v>8176737092</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>6</v>
+        <v>90</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>170</v>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="18" t="s">
+        <v>62</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>139</v>
+        <v>34</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>80</v>
+        <v>42</v>
+      </c>
+      <c r="E20" s="7">
+        <v>8177157999</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>56</v>
+        <v>103</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
-        <v>46</v>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>169</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E21" s="7">
-        <v>2146636606</v>
+        <v>54</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="G21" s="5"/>
+        <v>55</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>56</v>
+      </c>
       <c r="H21" s="5"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
-        <v>148</v>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="17" t="s">
+        <v>46</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E22" s="7">
-        <v>8179413620</v>
+        <v>2146636606</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>106</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
-        <v>62</v>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="19" t="s">
+        <v>147</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>165</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E23" s="7">
-        <v>2143340050</v>
+        <v>8179413620</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
+        <v>96</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>106</v>
+      </c>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I24" s="5"/>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" s="7">
+        <v>2143340050</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="6"/>
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -1778,7 +1810,7 @@
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -1791,578 +1823,574 @@
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G42" s="1"/>
     </row>
-    <row r="43" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G43" s="1"/>
     </row>
-    <row r="44" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G46" s="1"/>
     </row>
-    <row r="47" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G48" s="1"/>
     </row>
-    <row r="49" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G49" s="1"/>
     </row>
-    <row r="50" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G50" s="1"/>
     </row>
-    <row r="51" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G51" s="1"/>
     </row>
-    <row r="52" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G52" s="1"/>
     </row>
-    <row r="53" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G53" s="1"/>
     </row>
-    <row r="54" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G54" s="1"/>
     </row>
-    <row r="55" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G55" s="1"/>
     </row>
-    <row r="56" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G56" s="1"/>
     </row>
-    <row r="57" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G57" s="1"/>
     </row>
-    <row r="58" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G58" s="1"/>
     </row>
-    <row r="59" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G59" s="1"/>
     </row>
-    <row r="60" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G60" s="1"/>
     </row>
-    <row r="61" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G61" s="1"/>
     </row>
-    <row r="62" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G62" s="1"/>
     </row>
-    <row r="63" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G63" s="1"/>
     </row>
-    <row r="64" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G64" s="1"/>
     </row>
-    <row r="65" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G65" s="1"/>
     </row>
-    <row r="66" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G66" s="1"/>
     </row>
-    <row r="67" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G67" s="1"/>
     </row>
-    <row r="68" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G68" s="1"/>
     </row>
-    <row r="69" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G69" s="1"/>
     </row>
-    <row r="70" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G70" s="1"/>
     </row>
-    <row r="71" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G71" s="1"/>
     </row>
-    <row r="72" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G72" s="1"/>
     </row>
-    <row r="73" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G73" s="1"/>
     </row>
-    <row r="74" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G74" s="1"/>
     </row>
-    <row r="75" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G75" s="1"/>
     </row>
-    <row r="76" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G76" s="1"/>
     </row>
-    <row r="77" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G77" s="1"/>
     </row>
-    <row r="78" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G78" s="1"/>
     </row>
-    <row r="79" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G79" s="1"/>
     </row>
-    <row r="80" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G80" s="1"/>
     </row>
-    <row r="81" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G81" s="1"/>
     </row>
-    <row r="82" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G82" s="1"/>
     </row>
-    <row r="83" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G83" s="1"/>
     </row>
-    <row r="84" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G84" s="1"/>
     </row>
-    <row r="85" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G85" s="1"/>
     </row>
-    <row r="86" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G86" s="1"/>
     </row>
-    <row r="87" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G87" s="1"/>
     </row>
-    <row r="88" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G88" s="1"/>
     </row>
-    <row r="89" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G89" s="1"/>
     </row>
-    <row r="90" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G90" s="1"/>
     </row>
-    <row r="91" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G91" s="1"/>
     </row>
-    <row r="92" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G92" s="1"/>
     </row>
-    <row r="93" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G93" s="1"/>
     </row>
-    <row r="94" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G94" s="1"/>
     </row>
-    <row r="95" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G95" s="1"/>
     </row>
-    <row r="96" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G96" s="1"/>
     </row>
-    <row r="97" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G97" s="1"/>
     </row>
-    <row r="98" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G98" s="1"/>
     </row>
-    <row r="99" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G99" s="1"/>
     </row>
-    <row r="100" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G100" s="1"/>
     </row>
-    <row r="101" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G101" s="1"/>
     </row>
-    <row r="102" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G102" s="1"/>
     </row>
-    <row r="103" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G103" s="1"/>
     </row>
-    <row r="104" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G104" s="1"/>
     </row>
-    <row r="105" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G105" s="1"/>
     </row>
-    <row r="106" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G106" s="1"/>
     </row>
-    <row r="107" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G107" s="1"/>
     </row>
-    <row r="108" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G108" s="1"/>
     </row>
-    <row r="109" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G109" s="1"/>
     </row>
-    <row r="110" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G110" s="1"/>
     </row>
-    <row r="111" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G111" s="1"/>
     </row>
-    <row r="112" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G112" s="1"/>
     </row>
-    <row r="113" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G113" s="1"/>
     </row>
-    <row r="114" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G114" s="1"/>
     </row>
-    <row r="115" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G115" s="1"/>
     </row>
-    <row r="116" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G116" s="1"/>
     </row>
-    <row r="117" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G117" s="1"/>
     </row>
-    <row r="118" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G118" s="1"/>
     </row>
-    <row r="119" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G119" s="1"/>
     </row>
-    <row r="120" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G120" s="1"/>
     </row>
-    <row r="121" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G121" s="1"/>
     </row>
-    <row r="122" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G122" s="1"/>
     </row>
-    <row r="123" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G123" s="1"/>
     </row>
-    <row r="124" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G124" s="1"/>
     </row>
-    <row r="125" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G125" s="1"/>
     </row>
-    <row r="126" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G126" s="1"/>
     </row>
-    <row r="127" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G127" s="1"/>
     </row>
-    <row r="128" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G128" s="1"/>
     </row>
-    <row r="129" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G129" s="1"/>
     </row>
-    <row r="130" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G130" s="1"/>
     </row>
-    <row r="131" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G131" s="1"/>
     </row>
-    <row r="132" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G132" s="1"/>
     </row>
-    <row r="133" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G133" s="1"/>
     </row>
-    <row r="134" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G134" s="1"/>
     </row>
-    <row r="135" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G135" s="1"/>
     </row>
-    <row r="136" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G136" s="1"/>
     </row>
-    <row r="137" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G137" s="1"/>
     </row>
-    <row r="138" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G138" s="1"/>
     </row>
-    <row r="139" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G139" s="1"/>
     </row>
-    <row r="140" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G140" s="1"/>
     </row>
-    <row r="141" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G141" s="1"/>
     </row>
-    <row r="142" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G142" s="1"/>
     </row>
-    <row r="143" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G143" s="1"/>
     </row>
-    <row r="144" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G144" s="1"/>
     </row>
-    <row r="145" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G145" s="1"/>
     </row>
-    <row r="146" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G146" s="1"/>
     </row>
-    <row r="147" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G147" s="1"/>
     </row>
-    <row r="148" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G148" s="1"/>
     </row>
-    <row r="149" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G149" s="1"/>
     </row>
-    <row r="150" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G150" s="1"/>
     </row>
-    <row r="151" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G151" s="1"/>
     </row>
-    <row r="152" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G152" s="1"/>
     </row>
-    <row r="153" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G153" s="1"/>
     </row>
-    <row r="154" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G154" s="1"/>
     </row>
-    <row r="155" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G155" s="1"/>
     </row>
-    <row r="156" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G156" s="1"/>
     </row>
-    <row r="157" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G157" s="1"/>
     </row>
-    <row r="158" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G158" s="1"/>
     </row>
-    <row r="159" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G159" s="1"/>
     </row>
-    <row r="160" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G160" s="1"/>
     </row>
-    <row r="161" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G161" s="1"/>
     </row>
-    <row r="162" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G162" s="1"/>
     </row>
-    <row r="163" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G163" s="1"/>
     </row>
-    <row r="164" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G164" s="1"/>
     </row>
-    <row r="165" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G165" s="1"/>
     </row>
-    <row r="166" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G166" s="1"/>
     </row>
-    <row r="167" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G167" s="1"/>
     </row>
-    <row r="168" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G168" s="1"/>
     </row>
-    <row r="169" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G169" s="1"/>
     </row>
-    <row r="170" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G170" s="1"/>
     </row>
-    <row r="171" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G171" s="1"/>
     </row>
-    <row r="172" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G172" s="1"/>
     </row>
-    <row r="173" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G173" s="1"/>
     </row>
-    <row r="174" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G174" s="1"/>
     </row>
-    <row r="175" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G175" s="1"/>
     </row>
-    <row r="176" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G176" s="1"/>
     </row>
-    <row r="177" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G177" s="1"/>
     </row>
-    <row r="178" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G178" s="1"/>
     </row>
-    <row r="179" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G179" s="1"/>
     </row>
-    <row r="180" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G180" s="1"/>
     </row>
-    <row r="181" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G181" s="1"/>
     </row>
-    <row r="182" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G182" s="1"/>
     </row>
-    <row r="183" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G183" s="1"/>
     </row>
-    <row r="184" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G184" s="1"/>
     </row>
-    <row r="185" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G185" s="1"/>
     </row>
-    <row r="186" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G186" s="1"/>
     </row>
-    <row r="187" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G187" s="1"/>
     </row>
-    <row r="188" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G188" s="1"/>
     </row>
-    <row r="189" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G189" s="1"/>
     </row>
-    <row r="190" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G190" s="1"/>
     </row>
-    <row r="191" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G191" s="1"/>
     </row>
-    <row r="192" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G192" s="1"/>
     </row>
-    <row r="193" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G193" s="1"/>
     </row>
-    <row r="194" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="194" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G194" s="1"/>
     </row>
-    <row r="195" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="195" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G195" s="1"/>
     </row>
-    <row r="196" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G196" s="1"/>
     </row>
-    <row r="197" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G197" s="1"/>
     </row>
-    <row r="198" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="198" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G198" s="1"/>
     </row>
-    <row r="199" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G199" s="1"/>
-    </row>
-    <row r="200" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G200" s="1"/>
-    </row>
-    <row r="201" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G201" s="1"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:K201">
-    <sortCondition ref="B1:B201"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K199">
+    <sortCondition ref="B2:B199"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{D546FA9A-DF78-48C0-BA00-9866A3726FAE}"/>
-    <hyperlink ref="G2" r:id="rId2" xr:uid="{BBF483FB-AB08-490B-BC4F-8BFAC9BC8AAF}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{8B4B0520-EB2F-43BC-A19E-29548C846D2D}"/>
-    <hyperlink ref="G4" r:id="rId4" xr:uid="{A0B910A5-2E2B-4BC7-910D-FA4E7D80E148}"/>
-    <hyperlink ref="G5" r:id="rId5" xr:uid="{EE33A8E2-B273-4FB8-924E-EC84030BAE39}"/>
-    <hyperlink ref="F6" r:id="rId6" xr:uid="{6B3AA6BC-7EE4-48C5-8152-D0534A6D7FB7}"/>
-    <hyperlink ref="G7" r:id="rId7" xr:uid="{B1660469-60C4-4E54-BCA5-F93CF5D18B6D}"/>
-    <hyperlink ref="F20" r:id="rId8" xr:uid="{04BC0C7C-964B-42D9-A73C-B6627B954140}"/>
-    <hyperlink ref="G20" r:id="rId9" xr:uid="{479A147C-7FE7-4E3E-933A-4098CFE476B5}"/>
-    <hyperlink ref="F9" r:id="rId10" xr:uid="{514AF0BA-D3B9-4B24-BE00-5BB133BD6D0E}"/>
-    <hyperlink ref="G9" r:id="rId11" xr:uid="{EA7FAB1F-1321-4CB0-B589-D1354ABDDB06}"/>
-    <hyperlink ref="F10" r:id="rId12" xr:uid="{6EB4FDC4-BF24-4351-9AF3-71AE034BF3BD}"/>
-    <hyperlink ref="F11" r:id="rId13" xr:uid="{4A30D9F3-C05A-4BEB-8C17-13A5D0CB08E3}"/>
-    <hyperlink ref="G11" r:id="rId14" xr:uid="{883FDD81-CBB1-4FE1-AF74-E6195825B5BB}"/>
-    <hyperlink ref="F12" r:id="rId15" xr:uid="{4734A5D8-54F4-4FEB-A0A2-E8DA137ED5DD}"/>
-    <hyperlink ref="G12" r:id="rId16" xr:uid="{B60FC6F4-422C-4868-8751-58EAC85AB3B7}"/>
-    <hyperlink ref="F13" r:id="rId17" xr:uid="{89CB12A4-5980-4E81-8D48-082CA3AD1569}"/>
-    <hyperlink ref="G13" r:id="rId18" xr:uid="{00563C47-A3D9-4F67-B978-A462A91B6DA1}"/>
-    <hyperlink ref="F15" r:id="rId19" xr:uid="{09230410-1A15-42CF-B32A-C2FF25BE15C5}"/>
-    <hyperlink ref="F16" r:id="rId20" xr:uid="{B15A6018-435D-4615-8FFF-084056249A0D}"/>
-    <hyperlink ref="F18" r:id="rId21" xr:uid="{0C2A553D-4C5A-4907-B45B-377C2F63AD11}"/>
-    <hyperlink ref="F21" r:id="rId22" xr:uid="{34C983F1-F901-4025-AE92-2C06342821C5}"/>
-    <hyperlink ref="F19" r:id="rId23" xr:uid="{E7D46562-D24D-463F-9088-530E3B0B71A1}"/>
-    <hyperlink ref="F23" r:id="rId24" xr:uid="{DABACCA9-706C-4C4F-AC21-BEC1C07A9815}"/>
-    <hyperlink ref="F22" r:id="rId25" xr:uid="{47F18E21-37F4-4CE9-A6F6-D4621EFFBA01}"/>
-    <hyperlink ref="F17" r:id="rId26" xr:uid="{CC10832A-C004-4A03-8E5F-6F16BB873F84}"/>
-    <hyperlink ref="G16" r:id="rId27" xr:uid="{EE8C6852-8A26-4F2F-B061-7103FE6843BB}"/>
-    <hyperlink ref="G18" r:id="rId28" xr:uid="{456020CC-8BF1-4E11-AF64-6BF872D455B6}"/>
-    <hyperlink ref="G19" r:id="rId29" xr:uid="{2F427FF0-80B9-439C-9DB8-3DAE1F2DA4A0}"/>
-    <hyperlink ref="G22" r:id="rId30" xr:uid="{D61F35B2-1241-452E-BEDE-EE2B02A8C326}"/>
-    <hyperlink ref="G8" r:id="rId31" xr:uid="{2D4D38EE-7A2B-4D53-BCFF-3B0C0345B1D2}"/>
-    <hyperlink ref="F1" r:id="rId32" xr:uid="{3C286FEE-57C3-41CE-B6B5-A58EAC42A544}"/>
-    <hyperlink ref="G1" r:id="rId33" xr:uid="{7E493C0D-7901-4F9F-ADB7-2BA96AE7A79E}"/>
-    <hyperlink ref="F3" r:id="rId34" xr:uid="{6A6F54B1-64B2-4567-84EB-05CAA1109E00}"/>
-    <hyperlink ref="F14" r:id="rId35" xr:uid="{B2FA0509-BC30-469F-AB9D-28755C8131A5}"/>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{D546FA9A-DF78-48C0-BA00-9866A3726FAE}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{BBF483FB-AB08-490B-BC4F-8BFAC9BC8AAF}"/>
+    <hyperlink ref="F5" r:id="rId3" xr:uid="{8B4B0520-EB2F-43BC-A19E-29548C846D2D}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{A0B910A5-2E2B-4BC7-910D-FA4E7D80E148}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{EE33A8E2-B273-4FB8-924E-EC84030BAE39}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{6B3AA6BC-7EE4-48C5-8152-D0534A6D7FB7}"/>
+    <hyperlink ref="G8" r:id="rId7" xr:uid="{B1660469-60C4-4E54-BCA5-F93CF5D18B6D}"/>
+    <hyperlink ref="F21" r:id="rId8" xr:uid="{04BC0C7C-964B-42D9-A73C-B6627B954140}"/>
+    <hyperlink ref="G21" r:id="rId9" xr:uid="{479A147C-7FE7-4E3E-933A-4098CFE476B5}"/>
+    <hyperlink ref="F10" r:id="rId10" xr:uid="{514AF0BA-D3B9-4B24-BE00-5BB133BD6D0E}"/>
+    <hyperlink ref="G10" r:id="rId11" xr:uid="{EA7FAB1F-1321-4CB0-B589-D1354ABDDB06}"/>
+    <hyperlink ref="F11" r:id="rId12" xr:uid="{6EB4FDC4-BF24-4351-9AF3-71AE034BF3BD}"/>
+    <hyperlink ref="F12" r:id="rId13" xr:uid="{4A30D9F3-C05A-4BEB-8C17-13A5D0CB08E3}"/>
+    <hyperlink ref="G12" r:id="rId14" xr:uid="{883FDD81-CBB1-4FE1-AF74-E6195825B5BB}"/>
+    <hyperlink ref="F13" r:id="rId15" xr:uid="{4734A5D8-54F4-4FEB-A0A2-E8DA137ED5DD}"/>
+    <hyperlink ref="G13" r:id="rId16" xr:uid="{B60FC6F4-422C-4868-8751-58EAC85AB3B7}"/>
+    <hyperlink ref="F14" r:id="rId17" xr:uid="{89CB12A4-5980-4E81-8D48-082CA3AD1569}"/>
+    <hyperlink ref="G14" r:id="rId18" xr:uid="{00563C47-A3D9-4F67-B978-A462A91B6DA1}"/>
+    <hyperlink ref="F16" r:id="rId19" xr:uid="{09230410-1A15-42CF-B32A-C2FF25BE15C5}"/>
+    <hyperlink ref="F17" r:id="rId20" xr:uid="{B15A6018-435D-4615-8FFF-084056249A0D}"/>
+    <hyperlink ref="F19" r:id="rId21" xr:uid="{0C2A553D-4C5A-4907-B45B-377C2F63AD11}"/>
+    <hyperlink ref="F22" r:id="rId22" xr:uid="{34C983F1-F901-4025-AE92-2C06342821C5}"/>
+    <hyperlink ref="F20" r:id="rId23" xr:uid="{E7D46562-D24D-463F-9088-530E3B0B71A1}"/>
+    <hyperlink ref="F24" r:id="rId24" xr:uid="{DABACCA9-706C-4C4F-AC21-BEC1C07A9815}"/>
+    <hyperlink ref="F23" r:id="rId25" xr:uid="{47F18E21-37F4-4CE9-A6F6-D4621EFFBA01}"/>
+    <hyperlink ref="F18" r:id="rId26" xr:uid="{CC10832A-C004-4A03-8E5F-6F16BB873F84}"/>
+    <hyperlink ref="G17" r:id="rId27" xr:uid="{EE8C6852-8A26-4F2F-B061-7103FE6843BB}"/>
+    <hyperlink ref="G19" r:id="rId28" xr:uid="{456020CC-8BF1-4E11-AF64-6BF872D455B6}"/>
+    <hyperlink ref="G20" r:id="rId29" xr:uid="{2F427FF0-80B9-439C-9DB8-3DAE1F2DA4A0}"/>
+    <hyperlink ref="G23" r:id="rId30" xr:uid="{D61F35B2-1241-452E-BEDE-EE2B02A8C326}"/>
+    <hyperlink ref="G9" r:id="rId31" xr:uid="{2D4D38EE-7A2B-4D53-BCFF-3B0C0345B1D2}"/>
+    <hyperlink ref="F2" r:id="rId32" xr:uid="{3C286FEE-57C3-41CE-B6B5-A58EAC42A544}"/>
+    <hyperlink ref="G2" r:id="rId33" xr:uid="{7E493C0D-7901-4F9F-ADB7-2BA96AE7A79E}"/>
+    <hyperlink ref="F4" r:id="rId34" xr:uid="{6A6F54B1-64B2-4567-84EB-05CAA1109E00}"/>
+    <hyperlink ref="F15" r:id="rId35" xr:uid="{B2FA0509-BC30-469F-AB9D-28755C8131A5}"/>
+    <hyperlink ref="F9" r:id="rId36" xr:uid="{E0149BB9-0A89-41D4-A399-3C4C7EB2A1BB}"/>
+    <hyperlink ref="F8" r:id="rId37" xr:uid="{013DFA03-4AD4-49EC-BE0A-2CE24138CC13}"/>
   </hyperlinks>
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0" right="0" top="1.5" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId36"/>
+  <pageSetup orientation="landscape" r:id="rId38"/>
   <headerFooter>
     <oddHeader>&amp;C
 NORTH TEXAS CLUBS AND RESPRESENTIVES</oddHeader>
@@ -2379,17 +2407,17 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="31.5703125" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="31.5546875" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2412,7 +2440,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -2433,7 +2461,7 @@
       </c>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -2454,7 +2482,7 @@
       </c>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
@@ -2475,7 +2503,7 @@
       </c>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -2496,7 +2524,7 @@
       </c>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
@@ -2517,7 +2545,7 @@
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>46</v>
       </c>
@@ -2538,7 +2566,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>48</v>
       </c>
@@ -2559,7 +2587,7 @@
       </c>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>50</v>
       </c>
@@ -2580,7 +2608,7 @@
       </c>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="5" t="s">
         <v>25</v>
@@ -2599,7 +2627,7 @@
       </c>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>61</v>
       </c>
@@ -2620,7 +2648,7 @@
       </c>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>63</v>
       </c>
@@ -2641,7 +2669,7 @@
         <v>1950</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>62</v>
       </c>
@@ -2662,7 +2690,7 @@
       </c>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>62</v>
       </c>
@@ -2683,7 +2711,7 @@
       </c>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="5" t="s">
         <v>29</v>
@@ -2700,7 +2728,7 @@
       </c>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>5</v>
       </c>
@@ -2719,7 +2747,7 @@
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>100</v>
       </c>
@@ -2742,7 +2770,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>5</v>
       </c>
@@ -2763,7 +2791,7 @@
       </c>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>46</v>
       </c>
@@ -2782,7 +2810,7 @@
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>62</v>
       </c>
@@ -2803,7 +2831,7 @@
       </c>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>48</v>
       </c>
@@ -2822,7 +2850,7 @@
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>104</v>
       </c>
@@ -2845,7 +2873,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>5</v>
       </c>
@@ -2862,7 +2890,7 @@
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="6"/>

</xml_diff>